<commit_message>
Adds briefs to main pipeline
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4963E0-BBFA-4B89-91D3-8C4D02A641E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F69A97-A4ED-4C26-AC21-A0C8EB977C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$132</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="404">
   <si>
     <t>name_portal</t>
   </si>
@@ -1222,6 +1235,30 @@
   </si>
   <si>
     <t>2022, November</t>
+  </si>
+  <si>
+    <t>Adulthood and Elderly</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>School-aged Children</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prenatal and Early Childhood </t>
+  </si>
+  <si>
+    <t>All Ages</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Youth</t>
   </si>
 </sst>
 </file>
@@ -1587,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,6 +1687,16 @@
       <c r="G2" t="s">
         <v>289</v>
       </c>
+      <c r="H2" t="s">
+        <v>396</v>
+      </c>
+      <c r="I2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J2">
+        <f>1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1673,6 +1720,16 @@
       <c r="G3" t="s">
         <v>187</v>
       </c>
+      <c r="H3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I3" t="s">
+        <v>399</v>
+      </c>
+      <c r="J3">
+        <f>J2+1</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1690,6 +1747,16 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
+      <c r="H4" t="s">
+        <v>400</v>
+      </c>
+      <c r="I4" t="s">
+        <v>397</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J67" si="0">J3+1</f>
+        <v>3</v>
+      </c>
       <c r="K4" t="s">
         <v>19</v>
       </c>
@@ -1710,6 +1777,16 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
+      <c r="H5" t="s">
+        <v>398</v>
+      </c>
+      <c r="I5" t="s">
+        <v>399</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="K5" t="s">
         <v>23</v>
       </c>
@@ -1730,6 +1807,13 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
+      <c r="H6" t="s">
+        <v>401</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="K6" t="s">
         <v>27</v>
       </c>
@@ -1744,6 +1828,13 @@
       <c r="C7" t="s">
         <v>217</v>
       </c>
+      <c r="H7" t="s">
+        <v>401</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="K7" t="s">
         <v>220</v>
       </c>
@@ -1767,6 +1858,13 @@
       <c r="G8" t="s">
         <v>294</v>
       </c>
+      <c r="H8" t="s">
+        <v>401</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1781,6 +1879,16 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
+      <c r="H9" t="s">
+        <v>400</v>
+      </c>
+      <c r="I9" t="s">
+        <v>397</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1795,6 +1903,16 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
+      <c r="H10" t="s">
+        <v>398</v>
+      </c>
+      <c r="I10" t="s">
+        <v>399</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1806,6 +1924,16 @@
       <c r="C11" t="s">
         <v>217</v>
       </c>
+      <c r="H11" t="s">
+        <v>396</v>
+      </c>
+      <c r="I11" t="s">
+        <v>402</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="K11" t="s">
         <v>220</v>
       </c>
@@ -1820,6 +1948,16 @@
       <c r="C12" t="s">
         <v>217</v>
       </c>
+      <c r="H12" t="s">
+        <v>396</v>
+      </c>
+      <c r="I12" t="s">
+        <v>402</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="K12" t="s">
         <v>232</v>
       </c>
@@ -1834,6 +1972,16 @@
       <c r="C13" t="s">
         <v>217</v>
       </c>
+      <c r="H13" t="s">
+        <v>396</v>
+      </c>
+      <c r="I13" t="s">
+        <v>402</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="K13" t="s">
         <v>220</v>
       </c>
@@ -1848,6 +1996,16 @@
       <c r="C14" t="s">
         <v>217</v>
       </c>
+      <c r="H14" t="s">
+        <v>396</v>
+      </c>
+      <c r="I14" t="s">
+        <v>402</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="K14" t="s">
         <v>232</v>
       </c>
@@ -1862,6 +2020,16 @@
       <c r="C15" t="s">
         <v>217</v>
       </c>
+      <c r="H15" t="s">
+        <v>396</v>
+      </c>
+      <c r="I15" t="s">
+        <v>402</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="K15" t="s">
         <v>228</v>
       </c>
@@ -1876,6 +2044,16 @@
       <c r="C16" t="s">
         <v>217</v>
       </c>
+      <c r="H16" t="s">
+        <v>396</v>
+      </c>
+      <c r="I16" t="s">
+        <v>402</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="K16" t="s">
         <v>222</v>
       </c>
@@ -1890,6 +2068,16 @@
       <c r="C17" t="s">
         <v>217</v>
       </c>
+      <c r="H17" t="s">
+        <v>403</v>
+      </c>
+      <c r="I17" t="s">
+        <v>402</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="K17" t="s">
         <v>234</v>
       </c>
@@ -1916,6 +2104,16 @@
       <c r="G18" t="s">
         <v>187</v>
       </c>
+      <c r="H18" t="s">
+        <v>403</v>
+      </c>
+      <c r="I18" t="s">
+        <v>402</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="K18" t="s">
         <v>191</v>
       </c>
@@ -1933,6 +2131,16 @@
       <c r="G19" t="s">
         <v>14</v>
       </c>
+      <c r="H19" t="s">
+        <v>403</v>
+      </c>
+      <c r="I19" t="s">
+        <v>402</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="K19" t="s">
         <v>15</v>
       </c>
@@ -1959,6 +2167,16 @@
       <c r="G20" t="s">
         <v>187</v>
       </c>
+      <c r="H20" t="s">
+        <v>403</v>
+      </c>
+      <c r="I20" t="s">
+        <v>402</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
       <c r="K20" t="s">
         <v>203</v>
       </c>
@@ -1985,6 +2203,16 @@
       <c r="G21" t="s">
         <v>187</v>
       </c>
+      <c r="H21" t="s">
+        <v>403</v>
+      </c>
+      <c r="I21" t="s">
+        <v>402</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
       <c r="K21" t="s">
         <v>203</v>
       </c>
@@ -2011,6 +2239,16 @@
       <c r="G22" t="s">
         <v>187</v>
       </c>
+      <c r="H22" t="s">
+        <v>403</v>
+      </c>
+      <c r="I22" t="s">
+        <v>402</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
       <c r="K22" t="s">
         <v>203</v>
       </c>
@@ -2031,6 +2269,16 @@
       <c r="G23" t="s">
         <v>14</v>
       </c>
+      <c r="H23" t="s">
+        <v>398</v>
+      </c>
+      <c r="I23" t="s">
+        <v>399</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2048,6 +2296,16 @@
       <c r="G24" t="s">
         <v>14</v>
       </c>
+      <c r="H24" t="s">
+        <v>401</v>
+      </c>
+      <c r="I24" t="s">
+        <v>399</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2068,6 +2326,16 @@
       <c r="G25" t="s">
         <v>14</v>
       </c>
+      <c r="H25" t="s">
+        <v>401</v>
+      </c>
+      <c r="I25" t="s">
+        <v>399</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2088,6 +2356,16 @@
       <c r="G26" t="s">
         <v>14</v>
       </c>
+      <c r="H26" t="s">
+        <v>400</v>
+      </c>
+      <c r="I26" t="s">
+        <v>399</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2108,6 +2386,16 @@
       <c r="G27" t="s">
         <v>14</v>
       </c>
+      <c r="H27" t="s">
+        <v>398</v>
+      </c>
+      <c r="I27" t="s">
+        <v>399</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2128,6 +2416,16 @@
       <c r="G28" t="s">
         <v>14</v>
       </c>
+      <c r="H28" t="s">
+        <v>398</v>
+      </c>
+      <c r="I28" t="s">
+        <v>399</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2148,6 +2446,16 @@
       <c r="G29" t="s">
         <v>14</v>
       </c>
+      <c r="H29" t="s">
+        <v>398</v>
+      </c>
+      <c r="I29" t="s">
+        <v>399</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2168,6 +2476,16 @@
       <c r="G30" t="s">
         <v>14</v>
       </c>
+      <c r="H30" t="s">
+        <v>398</v>
+      </c>
+      <c r="I30" t="s">
+        <v>399</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2188,6 +2506,16 @@
       <c r="G31" t="s">
         <v>14</v>
       </c>
+      <c r="H31" t="s">
+        <v>403</v>
+      </c>
+      <c r="I31" t="s">
+        <v>399</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2208,6 +2536,16 @@
       <c r="G32" t="s">
         <v>14</v>
       </c>
+      <c r="H32" t="s">
+        <v>401</v>
+      </c>
+      <c r="I32" t="s">
+        <v>397</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -2231,6 +2569,16 @@
       <c r="G33" t="s">
         <v>14</v>
       </c>
+      <c r="H33" t="s">
+        <v>401</v>
+      </c>
+      <c r="I33" t="s">
+        <v>397</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -2254,6 +2602,16 @@
       <c r="G34" t="s">
         <v>14</v>
       </c>
+      <c r="H34" t="s">
+        <v>398</v>
+      </c>
+      <c r="I34" t="s">
+        <v>399</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2277,6 +2635,16 @@
       <c r="G35" t="s">
         <v>352</v>
       </c>
+      <c r="H35" t="s">
+        <v>401</v>
+      </c>
+      <c r="I35" t="s">
+        <v>397</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2294,6 +2662,16 @@
       <c r="G36" t="s">
         <v>14</v>
       </c>
+      <c r="H36" t="s">
+        <v>401</v>
+      </c>
+      <c r="I36" t="s">
+        <v>397</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2317,6 +2695,16 @@
       <c r="G37" t="s">
         <v>14</v>
       </c>
+      <c r="H37" t="s">
+        <v>398</v>
+      </c>
+      <c r="I37" t="s">
+        <v>399</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="K37" t="s">
         <v>71</v>
       </c>
@@ -2343,6 +2731,16 @@
       <c r="G38" t="s">
         <v>14</v>
       </c>
+      <c r="H38" t="s">
+        <v>401</v>
+      </c>
+      <c r="I38" t="s">
+        <v>397</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
       <c r="K38" t="s">
         <v>71</v>
       </c>
@@ -2369,6 +2767,16 @@
       <c r="G39" t="s">
         <v>14</v>
       </c>
+      <c r="H39" t="s">
+        <v>401</v>
+      </c>
+      <c r="I39" t="s">
+        <v>397</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
       <c r="K39" t="s">
         <v>71</v>
       </c>
@@ -2395,6 +2803,16 @@
       <c r="G40" t="s">
         <v>14</v>
       </c>
+      <c r="H40" t="s">
+        <v>398</v>
+      </c>
+      <c r="I40" t="s">
+        <v>399</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
       <c r="K40" t="s">
         <v>71</v>
       </c>
@@ -2421,6 +2839,16 @@
       <c r="G41" t="s">
         <v>14</v>
       </c>
+      <c r="H41" t="s">
+        <v>400</v>
+      </c>
+      <c r="I41" t="s">
+        <v>397</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="K41" t="s">
         <v>71</v>
       </c>
@@ -2447,6 +2875,16 @@
       <c r="G42" t="s">
         <v>14</v>
       </c>
+      <c r="H42" t="s">
+        <v>400</v>
+      </c>
+      <c r="I42" t="s">
+        <v>397</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
       <c r="K42" t="s">
         <v>71</v>
       </c>
@@ -2473,6 +2911,16 @@
       <c r="G43" t="s">
         <v>14</v>
       </c>
+      <c r="H43" t="s">
+        <v>400</v>
+      </c>
+      <c r="I43" t="s">
+        <v>397</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
       <c r="K43" t="s">
         <v>71</v>
       </c>
@@ -2499,6 +2947,16 @@
       <c r="G44" t="s">
         <v>14</v>
       </c>
+      <c r="H44" t="s">
+        <v>400</v>
+      </c>
+      <c r="I44" t="s">
+        <v>397</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
       <c r="K44" t="s">
         <v>71</v>
       </c>
@@ -2525,6 +2983,16 @@
       <c r="G45" t="s">
         <v>14</v>
       </c>
+      <c r="H45" t="s">
+        <v>400</v>
+      </c>
+      <c r="I45" t="s">
+        <v>397</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
       <c r="K45" t="s">
         <v>71</v>
       </c>
@@ -2551,6 +3019,16 @@
       <c r="G46" t="s">
         <v>14</v>
       </c>
+      <c r="H46" t="s">
+        <v>403</v>
+      </c>
+      <c r="I46" t="s">
+        <v>397</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
       <c r="K46" t="s">
         <v>71</v>
       </c>
@@ -2577,6 +3055,16 @@
       <c r="G47" t="s">
         <v>14</v>
       </c>
+      <c r="H47" t="s">
+        <v>398</v>
+      </c>
+      <c r="I47" t="s">
+        <v>397</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
       <c r="K47" t="s">
         <v>71</v>
       </c>
@@ -2603,6 +3091,16 @@
       <c r="G48" t="s">
         <v>14</v>
       </c>
+      <c r="H48" t="s">
+        <v>400</v>
+      </c>
+      <c r="I48" t="s">
+        <v>397</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
       <c r="K48" t="s">
         <v>71</v>
       </c>
@@ -2629,6 +3127,16 @@
       <c r="G49" t="s">
         <v>352</v>
       </c>
+      <c r="H49" t="s">
+        <v>400</v>
+      </c>
+      <c r="I49" t="s">
+        <v>397</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -2640,6 +3148,16 @@
       <c r="C50" t="s">
         <v>217</v>
       </c>
+      <c r="H50" t="s">
+        <v>400</v>
+      </c>
+      <c r="I50" t="s">
+        <v>397</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
       <c r="K50" t="s">
         <v>271</v>
       </c>
@@ -2654,6 +3172,16 @@
       <c r="C51" t="s">
         <v>217</v>
       </c>
+      <c r="H51" t="s">
+        <v>400</v>
+      </c>
+      <c r="I51" t="s">
+        <v>397</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
       <c r="K51" t="s">
         <v>275</v>
       </c>
@@ -2668,6 +3196,16 @@
       <c r="C52" t="s">
         <v>217</v>
       </c>
+      <c r="H52" t="s">
+        <v>400</v>
+      </c>
+      <c r="I52" t="s">
+        <v>397</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
       <c r="K52" t="s">
         <v>279</v>
       </c>
@@ -2682,6 +3220,16 @@
       <c r="C53" t="s">
         <v>217</v>
       </c>
+      <c r="H53" t="s">
+        <v>400</v>
+      </c>
+      <c r="I53" t="s">
+        <v>397</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
       <c r="K53" t="s">
         <v>273</v>
       </c>
@@ -2696,6 +3244,16 @@
       <c r="C54" t="s">
         <v>217</v>
       </c>
+      <c r="H54" t="s">
+        <v>400</v>
+      </c>
+      <c r="I54" t="s">
+        <v>397</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
       <c r="K54" t="s">
         <v>283</v>
       </c>
@@ -2710,6 +3268,16 @@
       <c r="C55" t="s">
         <v>217</v>
       </c>
+      <c r="H55" t="s">
+        <v>400</v>
+      </c>
+      <c r="I55" t="s">
+        <v>397</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
       <c r="K55" t="s">
         <v>283</v>
       </c>
@@ -2724,6 +3292,16 @@
       <c r="C56" t="s">
         <v>217</v>
       </c>
+      <c r="H56" t="s">
+        <v>400</v>
+      </c>
+      <c r="I56" t="s">
+        <v>397</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
       <c r="K56" t="s">
         <v>218</v>
       </c>
@@ -2738,6 +3316,16 @@
       <c r="C57" t="s">
         <v>217</v>
       </c>
+      <c r="H57" t="s">
+        <v>400</v>
+      </c>
+      <c r="I57" t="s">
+        <v>397</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
       <c r="K57" t="s">
         <v>230</v>
       </c>
@@ -2764,6 +3352,16 @@
       <c r="G58" t="s">
         <v>14</v>
       </c>
+      <c r="H58" t="s">
+        <v>400</v>
+      </c>
+      <c r="I58" t="s">
+        <v>397</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -2787,6 +3385,16 @@
       <c r="G59" t="s">
         <v>14</v>
       </c>
+      <c r="H59" t="s">
+        <v>400</v>
+      </c>
+      <c r="I59" t="s">
+        <v>397</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -2810,6 +3418,16 @@
       <c r="G60" t="s">
         <v>14</v>
       </c>
+      <c r="H60" t="s">
+        <v>400</v>
+      </c>
+      <c r="I60" t="s">
+        <v>397</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -2833,6 +3451,16 @@
       <c r="G61" t="s">
         <v>14</v>
       </c>
+      <c r="H61" t="s">
+        <v>400</v>
+      </c>
+      <c r="I61" t="s">
+        <v>397</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -2856,6 +3484,16 @@
       <c r="G62" t="s">
         <v>14</v>
       </c>
+      <c r="H62" t="s">
+        <v>400</v>
+      </c>
+      <c r="I62" t="s">
+        <v>397</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -2879,6 +3517,16 @@
       <c r="G63" t="s">
         <v>14</v>
       </c>
+      <c r="H63" t="s">
+        <v>398</v>
+      </c>
+      <c r="I63" t="s">
+        <v>399</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2902,6 +3550,16 @@
       <c r="G64" t="s">
         <v>14</v>
       </c>
+      <c r="H64" t="s">
+        <v>403</v>
+      </c>
+      <c r="I64" t="s">
+        <v>397</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -2925,6 +3583,16 @@
       <c r="G65" t="s">
         <v>14</v>
       </c>
+      <c r="H65" t="s">
+        <v>401</v>
+      </c>
+      <c r="I65" t="s">
+        <v>397</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -2948,6 +3616,16 @@
       <c r="G66" t="s">
         <v>14</v>
       </c>
+      <c r="H66" t="s">
+        <v>400</v>
+      </c>
+      <c r="I66" t="s">
+        <v>397</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -2971,6 +3649,16 @@
       <c r="G67" t="s">
         <v>14</v>
       </c>
+      <c r="H67" t="s">
+        <v>401</v>
+      </c>
+      <c r="I67" t="s">
+        <v>397</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
       <c r="K67" t="s">
         <v>154</v>
       </c>
@@ -2997,6 +3685,16 @@
       <c r="G68" t="s">
         <v>14</v>
       </c>
+      <c r="H68" t="s">
+        <v>398</v>
+      </c>
+      <c r="I68" t="s">
+        <v>399</v>
+      </c>
+      <c r="J68">
+        <f t="shared" ref="J68:J74" si="1">J67+1</f>
+        <v>67</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -3020,6 +3718,16 @@
       <c r="G69" t="s">
         <v>14</v>
       </c>
+      <c r="H69" t="s">
+        <v>400</v>
+      </c>
+      <c r="I69" t="s">
+        <v>397</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -3043,6 +3751,16 @@
       <c r="G70" t="s">
         <v>187</v>
       </c>
+      <c r="H70" t="s">
+        <v>400</v>
+      </c>
+      <c r="I70" t="s">
+        <v>397</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
       <c r="K70" t="s">
         <v>195</v>
       </c>
@@ -3069,6 +3787,16 @@
       <c r="G71" t="s">
         <v>14</v>
       </c>
+      <c r="H71" t="s">
+        <v>398</v>
+      </c>
+      <c r="I71" t="s">
+        <v>399</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -3092,6 +3820,16 @@
       <c r="G72" t="s">
         <v>14</v>
       </c>
+      <c r="H72" t="s">
+        <v>398</v>
+      </c>
+      <c r="I72" t="s">
+        <v>399</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -3115,6 +3853,16 @@
       <c r="G73" t="s">
         <v>14</v>
       </c>
+      <c r="H73" t="s">
+        <v>398</v>
+      </c>
+      <c r="I73" t="s">
+        <v>399</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -3137,6 +3885,16 @@
       </c>
       <c r="G74" t="s">
         <v>14</v>
+      </c>
+      <c r="H74" t="s">
+        <v>403</v>
+      </c>
+      <c r="I74" t="s">
+        <v>399</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sets everything up for running pdf briefs
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255DEBD7-1AE4-4A83-9D6D-4DFDBABACFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96358663-0FB4-41DF-BFB9-527CA1BEF3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18975" yWindow="0" windowWidth="9825" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1388,7 +1388,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1401,6 +1401,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1441,18 +1449,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1756,8 +1767,8 @@
   <dimension ref="A1:K132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5224,7 +5235,7 @@
       <c r="F120" t="s">
         <v>339</v>
       </c>
-      <c r="G120" t="s">
+      <c r="G120" s="4" t="s">
         <v>340</v>
       </c>
       <c r="H120" t="s">
@@ -5612,6 +5623,9 @@
       <formula2>20</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G120" r:id="rId1" xr:uid="{86CF00EA-F175-49E3-B292-E21775BC70DA}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete remianing briefs texts
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="386" documentId="13_ncr:1_{29A47490-2D27-4D0C-B372-38E790C58E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2020AC11-4115-4A87-A5E7-A8822AF7785E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A4C604-F191-44FC-9A77-6FD34D6F47E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="501">
   <si>
     <t>name_portal</t>
   </si>
@@ -1348,9 +1348,6 @@
     <t>Institutional births</t>
   </si>
   <si>
-    <t>SRHINSTITUTIONALBIRTH</t>
-  </si>
-  <si>
     <t>The proportion of births occurring in health facilities in the area, or ‘institutional births’ or ‘institutional deliveries.</t>
   </si>
   <si>
@@ -1360,9 +1357,6 @@
     <t>Current education expenditure, total (% of total expenditure in public institutions)</t>
   </si>
   <si>
-    <t>SE.XPD.CTOT.ZS</t>
-  </si>
-  <si>
     <t>WDI</t>
   </si>
   <si>
@@ -1426,18 +1420,12 @@
     <t>out_school</t>
   </si>
   <si>
-    <t>OFST_1_CP</t>
-  </si>
-  <si>
     <t>4.6.2.Youth literacy rate, population 15-24 years, both sexes (%)</t>
   </si>
   <si>
     <t>The youth literacy rate is defined by the percentage of the population aged 15 to 24 years that can read and write. It is typically measured according to the ability to comprehend a short simple statement on everyday life. Generally, literacy also encompasses numeracy, and measurement may incorporate a simple assessment of arithmetic ability. </t>
   </si>
   <si>
-    <t>LR_Ag15t24.</t>
-  </si>
-  <si>
     <t>Early childbearing - percentage of women (aged 20-24 years) who gave birth before age 18</t>
   </si>
   <si>
@@ -1537,12 +1525,6 @@
     <t>IM_HPV</t>
   </si>
   <si>
-    <t>C040201</t>
-  </si>
-  <si>
-    <t>C040202</t>
-  </si>
-  <si>
     <t>DEMAny</t>
   </si>
   <si>
@@ -1565,6 +1547,9 @@
   </si>
   <si>
     <t>% of working-age population</t>
+  </si>
+  <si>
+    <t>rank 4</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1586,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1617,6 +1602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1649,7 +1640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1663,9 +1654,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1679,10 +1671,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1970,15 +1958,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L111" sqref="L111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
@@ -2019,7 +2006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>406</v>
       </c>
@@ -2051,7 +2038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>407</v>
       </c>
@@ -2083,7 +2070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>408</v>
       </c>
@@ -2118,7 +2105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>409</v>
       </c>
@@ -2199,7 +2186,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2222,7 +2209,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2248,7 +2235,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2274,7 +2261,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2300,7 +2287,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2326,7 +2313,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2352,7 +2339,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2381,7 +2368,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>410</v>
       </c>
@@ -2410,7 +2397,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -2433,7 +2420,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2468,7 +2455,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2500,7 +2487,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -2535,7 +2522,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2570,7 +2557,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -2602,7 +2589,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2634,7 +2621,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -2666,7 +2653,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
@@ -2698,7 +2685,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2730,7 +2717,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -2762,7 +2749,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -2794,7 +2781,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -2826,7 +2813,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -2855,7 +2842,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -2884,7 +2871,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -2913,7 +2900,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2945,7 +2932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>125</v>
       </c>
@@ -2974,7 +2961,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -3003,7 +2990,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>411</v>
       </c>
@@ -3035,7 +3022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -3064,7 +3051,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>138</v>
       </c>
@@ -3093,7 +3080,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>412</v>
       </c>
@@ -3128,7 +3115,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3157,7 +3144,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -3186,7 +3173,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>152</v>
       </c>
@@ -3215,7 +3202,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>156</v>
       </c>
@@ -3244,7 +3231,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>160</v>
       </c>
@@ -3273,7 +3260,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>164</v>
       </c>
@@ -3302,7 +3289,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -3334,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -3398,7 +3385,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -3462,7 +3449,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>190</v>
       </c>
@@ -3494,7 +3481,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>194</v>
       </c>
@@ -3526,7 +3513,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>197</v>
       </c>
@@ -3558,7 +3545,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>200</v>
       </c>
@@ -3622,7 +3609,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>206</v>
       </c>
@@ -3639,7 +3626,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -3659,7 +3646,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>211</v>
       </c>
@@ -3685,7 +3672,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>213</v>
       </c>
@@ -3705,7 +3692,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>214</v>
       </c>
@@ -3731,7 +3718,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>215</v>
       </c>
@@ -3757,7 +3744,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>217</v>
       </c>
@@ -3783,7 +3770,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>219</v>
       </c>
@@ -3803,7 +3790,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>221</v>
       </c>
@@ -3823,7 +3810,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>223</v>
       </c>
@@ -3849,7 +3836,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>225</v>
       </c>
@@ -3869,7 +3856,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>226</v>
       </c>
@@ -3967,7 +3954,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -4117,7 +4104,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>413</v>
       </c>
@@ -4143,7 +4130,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>414</v>
       </c>
@@ -4169,7 +4156,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>415</v>
       </c>
@@ -4195,7 +4182,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>416</v>
       </c>
@@ -4221,7 +4208,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>152</v>
       </c>
@@ -4273,7 +4260,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>260</v>
       </c>
@@ -4299,7 +4286,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>426</v>
       </c>
@@ -4325,7 +4312,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>264</v>
       </c>
@@ -4351,7 +4338,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>266</v>
       </c>
@@ -4403,7 +4390,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>268</v>
       </c>
@@ -4429,7 +4416,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>417</v>
       </c>
@@ -4559,7 +4546,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -4578,7 +4565,7 @@
       <c r="F93" t="s">
         <v>12</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="3" t="s">
         <v>278</v>
       </c>
       <c r="H93" t="s">
@@ -4620,7 +4607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>427</v>
       </c>
@@ -4649,7 +4636,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>427</v>
       </c>
@@ -4678,7 +4665,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>418</v>
       </c>
@@ -4713,7 +4700,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>419</v>
       </c>
@@ -4748,7 +4735,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>420</v>
       </c>
@@ -4780,7 +4767,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -4812,7 +4799,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>304</v>
       </c>
@@ -4847,7 +4834,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>308</v>
       </c>
@@ -4873,7 +4860,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>421</v>
       </c>
@@ -4908,7 +4895,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>422</v>
       </c>
@@ -4943,7 +4930,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>423</v>
       </c>
@@ -4975,7 +4962,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>424</v>
       </c>
@@ -5007,7 +4994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>327</v>
       </c>
@@ -5039,7 +5026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>331</v>
       </c>
@@ -5071,7 +5058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>335</v>
       </c>
@@ -5091,7 +5078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>337</v>
       </c>
@@ -5152,7 +5139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>342</v>
       </c>
@@ -5184,7 +5171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>345</v>
       </c>
@@ -5216,7 +5203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>349</v>
       </c>
@@ -5248,7 +5235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>425</v>
       </c>
@@ -5277,7 +5264,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>428</v>
       </c>
@@ -5306,7 +5293,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>429</v>
       </c>
@@ -5335,7 +5322,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>406</v>
       </c>
@@ -5370,24 +5357,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="C119" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="B119" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="D119" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="G119" s="6" t="s">
         <v>444</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="G119" s="6" t="s">
-        <v>446</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>369</v>
@@ -5399,21 +5386,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>497</v>
+        <v>447</v>
       </c>
       <c r="C120" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G120" s="6" t="s">
         <v>445</v>
-      </c>
-      <c r="D120" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="G120" s="6" t="s">
-        <v>447</v>
       </c>
       <c r="H120" s="5" t="s">
         <v>369</v>
@@ -5425,12 +5412,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>323</v>
@@ -5439,13 +5426,13 @@
         <v>432</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="G121" s="6" t="s">
         <v>434</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>435</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>369</v>
@@ -5457,27 +5444,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
+    <row r="122" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E122" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="B122" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="C122" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="D122" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="E122" s="5" t="s">
-        <v>442</v>
-      </c>
       <c r="F122" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H122" s="5" t="s">
         <v>377</v>
@@ -5485,28 +5472,30 @@
       <c r="I122" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="J122" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J122" s="9"/>
+      <c r="K122" s="9"/>
+      <c r="L122" s="9" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>12</v>
+        <v>479</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>479</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>377</v>
@@ -5515,24 +5504,24 @@
         <v>368</v>
       </c>
     </row>
-    <row r="124" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>12</v>
+        <v>477</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H124" s="5" t="s">
         <v>377</v>
@@ -5544,24 +5533,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>12</v>
+        <v>478</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>377</v>
@@ -5570,24 +5559,24 @@
         <v>368</v>
       </c>
     </row>
-    <row r="126" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>12</v>
+        <v>480</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H126" s="5" t="s">
         <v>377</v>
@@ -5596,24 +5585,24 @@
         <v>368</v>
       </c>
     </row>
-    <row r="127" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>12</v>
+        <v>481</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H127" s="5" t="s">
         <v>377</v>
@@ -5625,24 +5614,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>12</v>
+        <v>482</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H128" s="5" t="s">
         <v>377</v>
@@ -5652,26 +5641,26 @@
       </c>
     </row>
     <row r="129" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>458</v>
+      <c r="A129" s="9" t="s">
+        <v>456</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="C129" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C129" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="G129" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="E129" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F129" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="G129" s="6" t="s">
-        <v>457</v>
       </c>
       <c r="H129" s="5" t="s">
         <v>377</v>
@@ -5685,25 +5674,25 @@
     </row>
     <row r="130" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>462</v>
+        <v>488</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>488</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H130" s="5" t="s">
         <v>386</v>
@@ -5715,27 +5704,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F131" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>386</v>
@@ -5744,27 +5733,27 @@
         <v>370</v>
       </c>
     </row>
-    <row r="132" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>336</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H132" s="5" t="s">
         <v>386</v>
@@ -5776,27 +5765,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F133" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>386</v>
@@ -5808,27 +5797,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B134" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="D134" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="D134" s="5" t="s">
-        <v>480</v>
-      </c>
       <c r="E134" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H134" s="5" t="s">
         <v>394</v>
@@ -5840,21 +5829,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="H135" s="5" t="s">
         <v>394</v>
@@ -5866,7 +5855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:12" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>214</v>
       </c>
@@ -5877,10 +5866,10 @@
         <v>207</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="H136" s="8" t="s">
         <v>394</v>
@@ -5892,26 +5881,20 @@
         <v>1</v>
       </c>
       <c r="K136" s="8" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="L136" s="8" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K136" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Education"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K136" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G53" xr:uid="{2F5F9FA7-5446-47AF-A091-DD36F3BEED45}">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A218 B136" xr:uid="{C9CEA4D8-9D09-46A7-AFBC-6B7076AE134A}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A218 B136 B119:B130" xr:uid="{C9CEA4D8-9D09-46A7-AFBC-6B7076AE134A}">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
@@ -5931,8 +5914,9 @@
     <hyperlink ref="G133" r:id="rId12" xr:uid="{4223E1D3-2634-4817-9EFA-3F96BE143230}"/>
     <hyperlink ref="G11" r:id="rId13" xr:uid="{7F719CB2-8B34-4A47-8AB2-11A150ECAA5B}"/>
     <hyperlink ref="G94" r:id="rId14" xr:uid="{40D76283-D72C-4222-8FB8-B4531115EFAD}"/>
+    <hyperlink ref="G93" r:id="rId15" xr:uid="{6785D54E-5D95-47C1-AE62-5F24578C8401}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix order bug that showed missing data in the first indicator
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9A1520-E134-485D-94BE-58C789987881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB20E77-FE36-4EDA-82F4-1630D4E88F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="18975" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2136,9 +2136,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I69" sqref="I69"/>
+      <selection pane="topRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3397,7 +3397,9 @@
       <c r="I39" t="s">
         <v>382</v>
       </c>
-      <c r="J39"/>
+      <c r="J39">
+        <v>0</v>
+      </c>
       <c r="K39" t="s">
         <v>191</v>
       </c>
@@ -3429,6 +3431,9 @@
       </c>
       <c r="I40" t="s">
         <v>382</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
       </c>
       <c r="K40" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Add listings for data portal and UHCI in main db
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB20E77-FE36-4EDA-82F4-1630D4E88F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2C9288-8A66-4053-A636-819A3E74D826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="18975" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="563">
   <si>
     <t>name_portal</t>
   </si>
@@ -1724,6 +1724,18 @@
   </si>
   <si>
     <t>HVA_EPI_INF_RT_10_19</t>
+  </si>
+  <si>
+    <t>uhci</t>
+  </si>
+  <si>
+    <t>HD Chief Economist Office</t>
+  </si>
+  <si>
+    <t>Utilization-adjusted Capital Index (UHCI)</t>
+  </si>
+  <si>
+    <t>Basic measure of Utilization Adjusted Human Capital Index, defined as the Basic Utilization Rate (employment-to-working population ratio of the 15-64 age group) multiplied by the Human Capital Index (HCI).</t>
   </si>
 </sst>
 </file>
@@ -1760,7 +1772,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1782,6 +1794,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1814,7 +1832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1831,6 +1849,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2134,11 +2153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K137"/>
+  <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M13" sqref="M13"/>
+      <selection pane="topRight" activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6553,6 +6572,35 @@
         <v>1</v>
       </c>
       <c r="K137" s="5"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>559</v>
+      </c>
+      <c r="B138" t="s">
+        <v>559</v>
+      </c>
+      <c r="C138" t="s">
+        <v>560</v>
+      </c>
+      <c r="D138" t="s">
+        <v>561</v>
+      </c>
+      <c r="E138" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="F138" t="s">
+        <v>174</v>
+      </c>
+      <c r="H138" t="s">
+        <v>392</v>
+      </c>
+      <c r="I138" t="s">
+        <v>382</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K137" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Incorporate code for comp_data
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FC2C9288-8A66-4053-A636-819A3E74D826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{661EC13F-FF58-439C-B7C3-50311394597A}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{FC2C9288-8A66-4053-A636-819A3E74D826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B766D8E6-2AAE-4CC9-B26E-E3CADBDFCBBF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="565">
   <si>
     <t>name_portal</t>
   </si>
@@ -1737,11 +1737,20 @@
   <si>
     <t>Basic measure of Utilization Adjusted Human Capital Index, defined as the Basic Utilization Rate (employment-to-working population ratio of the 15-64 age group) multiplied by the Human Capital Index (HCI).</t>
   </si>
+  <si>
+    <t>Date_download</t>
+  </si>
+  <si>
+    <t>May 19, 2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1804,7 +1813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1827,12 +1836,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1850,9 +1870,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2157,20 +2181,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K138"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J105" sqref="J105"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="157" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2204,8 +2229,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>274</v>
       </c>
@@ -2236,8 +2264,11 @@
       <c r="J2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="14" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2263,7 +2294,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2289,7 +2320,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -2318,7 +2349,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2347,7 +2378,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -2379,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>415</v>
       </c>
@@ -2414,7 +2445,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>418</v>
       </c>
@@ -2449,7 +2480,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>416</v>
       </c>
@@ -2484,7 +2515,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>419</v>
       </c>
@@ -2519,7 +2550,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>417</v>
       </c>
@@ -2551,7 +2582,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>420</v>
       </c>
@@ -2583,7 +2614,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>458</v>
       </c>
@@ -2614,7 +2645,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>412</v>
       </c>
@@ -2649,7 +2680,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>411</v>
       </c>
@@ -3695,7 +3726,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>407</v>
       </c>
@@ -3724,7 +3755,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>421</v>
       </c>
@@ -3756,7 +3787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -3781,8 +3812,11 @@
       <c r="I51" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>436</v>
       </c>
@@ -3815,7 +3849,7 @@
       </c>
       <c r="K52" s="5"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>325</v>
       </c>
@@ -3847,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>120</v>
       </c>
@@ -3879,7 +3913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -3908,7 +3942,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>258</v>
       </c>
@@ -3943,7 +3977,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>262</v>
       </c>
@@ -3978,7 +4012,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>266</v>
       </c>
@@ -4013,7 +4047,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>272</v>
       </c>
@@ -4048,7 +4082,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>273</v>
       </c>
@@ -4083,7 +4117,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>204</v>
       </c>
@@ -4115,7 +4149,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>217</v>
       </c>
@@ -4147,7 +4181,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>413</v>
       </c>
@@ -4182,7 +4216,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>464</v>
       </c>
@@ -4704,7 +4738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>445</v>
       </c>
@@ -4737,7 +4771,7 @@
       </c>
       <c r="K81" s="5"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>137</v>
       </c>
@@ -4766,7 +4800,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>454</v>
       </c>
@@ -4799,7 +4833,7 @@
       </c>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>163</v>
       </c>
@@ -4828,7 +4862,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>333</v>
       </c>
@@ -4857,7 +4891,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>423</v>
       </c>
@@ -4892,7 +4926,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>198</v>
       </c>
@@ -4927,7 +4961,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>201</v>
       </c>
@@ -4962,7 +4996,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>335</v>
       </c>
@@ -4993,8 +5027,11 @@
       <c r="J89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>337</v>
       </c>
@@ -5026,7 +5063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>252</v>
       </c>
@@ -5061,7 +5098,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>159</v>
       </c>
@@ -5090,7 +5127,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>424</v>
       </c>
@@ -5119,7 +5156,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>424</v>
       </c>
@@ -5148,7 +5185,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>264</v>
       </c>
@@ -5183,7 +5220,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>403</v>
       </c>
@@ -6607,11 +6644,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K137" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K137">
-      <sortCondition ref="A1:A137"/>
-    </sortState>
-  </autoFilter>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G54" xr:uid="{2F5F9FA7-5446-47AF-A091-DD36F3BEED45}">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
Drop income comparison and change UHCI text
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{781CE06E-903C-4B18-9F3C-8462F60114A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C0963F6-59D3-482C-80DF-7926734AF803}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{781CE06E-903C-4B18-9F3C-8462F60114A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4EDCA12-F362-4DE9-BEEE-313A507D8CCB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1735,9 +1735,6 @@
     <t>Labor force participation (%), ages 25+</t>
   </si>
   <si>
-    <t>Survival Rate ( ages 15-60)</t>
-  </si>
-  <si>
     <t>Minimum proficiency in mathematics, primary (%)</t>
   </si>
   <si>
@@ -1975,6 +1972,9 @@
   </si>
   <si>
     <t>eap_dwap_mf_a</t>
+  </si>
+  <si>
+    <t>Survival Rate, ages 15-60 (%)</t>
   </si>
 </sst>
 </file>
@@ -2451,7 +2451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L4" sqref="L4"/>
+      <selection pane="topRight" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,10 +2653,10 @@
         <v>141</v>
       </c>
       <c r="D7" t="s">
-        <v>553</v>
+        <v>629</v>
       </c>
       <c r="E7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2688,7 +2688,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E8" t="s">
         <v>230</v>
@@ -2723,7 +2723,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E9" t="s">
         <v>250</v>
@@ -2758,7 +2758,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E10" t="s">
         <v>234</v>
@@ -2793,7 +2793,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E11" t="s">
         <v>253</v>
@@ -2828,7 +2828,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E12" t="s">
         <v>236</v>
@@ -2860,7 +2860,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E13" t="s">
         <v>255</v>
@@ -2958,7 +2958,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>448</v>
@@ -2987,7 +2987,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E17" t="s">
         <v>113</v>
@@ -3019,7 +3019,7 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E18" t="s">
         <v>447</v>
@@ -3054,7 +3054,7 @@
         <v>346</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>11</v>
@@ -3087,7 +3087,7 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E20" t="s">
         <v>139</v>
@@ -3119,7 +3119,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E21" t="s">
         <v>402</v>
@@ -3139,10 +3139,10 @@
     </row>
     <row r="22" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>379</v>
@@ -3186,10 +3186,10 @@
         <v>224</v>
       </c>
       <c r="D23" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E23" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>225</v>
@@ -3453,7 +3453,7 @@
         <v>379</v>
       </c>
       <c r="D31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E31" t="s">
         <v>392</v>
@@ -3491,10 +3491,10 @@
         <v>379</v>
       </c>
       <c r="D32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E32" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F32" t="s">
         <v>445</v>
@@ -3529,10 +3529,10 @@
         <v>379</v>
       </c>
       <c r="D33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F33" t="s">
         <v>445</v>
@@ -3570,7 +3570,7 @@
         <v>145</v>
       </c>
       <c r="E34" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F34" t="s">
         <v>142</v>
@@ -3716,7 +3716,7 @@
         <v>156</v>
       </c>
       <c r="E38" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F38" t="s">
         <v>142</v>
@@ -3754,7 +3754,7 @@
         <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F39" t="s">
         <v>142</v>
@@ -3789,7 +3789,7 @@
         <v>341</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5" t="s">
@@ -3823,7 +3823,7 @@
         <v>379</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>370</v>
@@ -3885,7 +3885,7 @@
         <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E43" t="s">
         <v>35</v>
@@ -3940,7 +3940,7 @@
         <v>346</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>367</v>
@@ -4057,7 +4057,7 @@
         <v>257</v>
       </c>
       <c r="D49" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E49" t="s">
         <v>258</v>
@@ -4121,7 +4121,7 @@
         <v>257</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>337</v>
@@ -4153,7 +4153,7 @@
         <v>257</v>
       </c>
       <c r="D52" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E52" t="s">
         <v>480</v>
@@ -4188,7 +4188,7 @@
         <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E53" t="s">
         <v>106</v>
@@ -4249,7 +4249,7 @@
         <v>141</v>
       </c>
       <c r="D55" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E55" t="s">
         <v>411</v>
@@ -4325,7 +4325,7 @@
         <v>141</v>
       </c>
       <c r="D57" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E57" t="s">
         <v>417</v>
@@ -4398,7 +4398,7 @@
         <v>141</v>
       </c>
       <c r="D59" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E59" t="s">
         <v>426</v>
@@ -4506,7 +4506,7 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E62" t="s">
         <v>406</v>
@@ -4541,7 +4541,7 @@
         <v>267</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>363</v>
@@ -4577,7 +4577,7 @@
         <v>224</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5" t="s">
@@ -4675,7 +4675,7 @@
         <v>224</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5" t="s">
@@ -4918,7 +4918,7 @@
         <v>12</v>
       </c>
       <c r="D75" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E75" t="s">
         <v>310</v>
@@ -4953,7 +4953,7 @@
         <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E76" t="s">
         <v>311</v>
@@ -5017,10 +5017,10 @@
         <v>141</v>
       </c>
       <c r="D78" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E78" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F78" t="s">
         <v>142</v>
@@ -5055,7 +5055,7 @@
         <v>257</v>
       </c>
       <c r="D79" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E79" t="s">
         <v>264</v>
@@ -5090,7 +5090,7 @@
         <v>12</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>421</v>
@@ -5113,7 +5113,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>116</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>494</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F81" t="s">
         <v>45</v>
@@ -5248,7 +5248,7 @@
         <v>141</v>
       </c>
       <c r="D85" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E85" t="s">
         <v>412</v>
@@ -5286,10 +5286,10 @@
         <v>141</v>
       </c>
       <c r="D86" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E86" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F86" t="s">
         <v>142</v>
@@ -5394,7 +5394,7 @@
         <v>396</v>
       </c>
       <c r="D89" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E89" t="s">
         <v>271</v>
@@ -5429,7 +5429,7 @@
         <v>141</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E90" s="13" t="s">
         <v>202</v>
@@ -5592,7 +5592,7 @@
         <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E95" t="s">
         <v>290</v>
@@ -5659,7 +5659,7 @@
         <v>257</v>
       </c>
       <c r="D97" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E97" t="s">
         <v>273</v>
@@ -5694,10 +5694,10 @@
         <v>141</v>
       </c>
       <c r="D98" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F98" t="s">
         <v>142</v>
@@ -5732,7 +5732,7 @@
         <v>257</v>
       </c>
       <c r="D99" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E99" t="s">
         <v>275</v>
@@ -5767,7 +5767,7 @@
         <v>257</v>
       </c>
       <c r="D100" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E100" t="s">
         <v>278</v>
@@ -5834,7 +5834,7 @@
         <v>436</v>
       </c>
       <c r="D102" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>437</v>
@@ -5866,7 +5866,7 @@
         <v>141</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E103" t="s">
         <v>423</v>
@@ -5904,7 +5904,7 @@
         <v>141</v>
       </c>
       <c r="D104" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E104" t="s">
         <v>415</v>
@@ -5942,7 +5942,7 @@
         <v>396</v>
       </c>
       <c r="D105" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E105" t="s">
         <v>394</v>
@@ -6015,7 +6015,7 @@
         <v>141</v>
       </c>
       <c r="D107" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E107" t="s">
         <v>424</v>
@@ -6205,7 +6205,7 @@
         <v>396</v>
       </c>
       <c r="D112" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E112" t="s">
         <v>400</v>
@@ -6348,7 +6348,7 @@
         <v>379</v>
       </c>
       <c r="D116" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E116" t="s">
         <v>476</v>
@@ -6386,7 +6386,7 @@
         <v>379</v>
       </c>
       <c r="D117" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E117" t="s">
         <v>476</v>
@@ -6456,7 +6456,7 @@
         <v>12</v>
       </c>
       <c r="D119" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E119" t="s">
         <v>244</v>
@@ -6517,7 +6517,7 @@
         <v>12</v>
       </c>
       <c r="D121" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E121" t="s">
         <v>51</v>
@@ -6552,7 +6552,7 @@
         <v>12</v>
       </c>
       <c r="D122" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E122" t="s">
         <v>56</v>
@@ -6584,7 +6584,7 @@
         <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E123" t="s">
         <v>60</v>
@@ -6619,7 +6619,7 @@
         <v>12</v>
       </c>
       <c r="D124" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E124" t="s">
         <v>63</v>
@@ -6939,7 +6939,7 @@
         <v>379</v>
       </c>
       <c r="D134" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E134" t="s">
         <v>427</v>
@@ -6974,7 +6974,7 @@
         <v>224</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>359</v>
@@ -7010,7 +7010,7 @@
         <v>396</v>
       </c>
       <c r="D136" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E136" t="s">
         <v>11</v>
@@ -7118,7 +7118,7 @@
         <v>141</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>538</v>
@@ -7154,7 +7154,7 @@
         <v>221</v>
       </c>
       <c r="D140" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E140" t="s">
         <v>541</v>
@@ -7189,7 +7189,7 @@
         <v>221</v>
       </c>
       <c r="D141" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E141" t="s">
         <v>543</v>
@@ -7224,7 +7224,7 @@
         <v>221</v>
       </c>
       <c r="D142" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E142" t="s">
         <v>545</v>

</xml_diff>

<commit_message>
Fix error with eap_2wap indicator ILO
Use modelled estimates from ILO
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{854E69F1-9186-4698-9780-F77BE94E82F4}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB464E23-119A-41D2-9A4B-AA629B74E7F7}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="390" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="711">
   <si>
     <t>name_portal</t>
   </si>
@@ -2153,6 +2153,33 @@
   </si>
   <si>
     <t>SDGSUICIDE</t>
+  </si>
+  <si>
+    <t>EIP_2WAP_SEX_AGE_RT_A_a</t>
+  </si>
+  <si>
+    <t>EIP_2WAP_SEX_AGE_RT_A_y</t>
+  </si>
+  <si>
+    <t>EIP_NEET_SEX_AGE_RT_A</t>
+  </si>
+  <si>
+    <t>EMP_NIFL_SEX_AGE_RT_A_a</t>
+  </si>
+  <si>
+    <t>EMP_NIFL_SEX_AGE_RT_A_y</t>
+  </si>
+  <si>
+    <t>LUU_2LU4_SEX_AGE_RT_A_a</t>
+  </si>
+  <si>
+    <t>LUU_2LU4_SEX_AGE_RT_A_y</t>
+  </si>
+  <si>
+    <t>UNE_2EAP_SEX_AGE_RT_A_a</t>
+  </si>
+  <si>
+    <t>UNE_2EAP_SEX_AGE_RT_A_y</t>
   </si>
 </sst>
 </file>
@@ -2612,7 +2639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D74" sqref="C74:D143"/>
+      <selection pane="topRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3150,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -3191,12 +3218,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>704</v>
       </c>
       <c r="C15" t="s">
         <v>369</v>
@@ -3747,12 +3774,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>709</v>
       </c>
       <c r="C29" t="s">
         <v>369</v>
@@ -3788,12 +3815,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>176</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>710</v>
       </c>
       <c r="C30" t="s">
         <v>369</v>
@@ -3905,12 +3932,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>163</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>705</v>
       </c>
       <c r="C33" t="s">
         <v>369</v>
@@ -4107,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>417</v>
       </c>
@@ -4262,12 +4289,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>173</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>706</v>
       </c>
       <c r="C42" t="s">
         <v>369</v>
@@ -4303,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>419</v>
       </c>
@@ -4622,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>591</v>
       </c>
@@ -5541,7 +5568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>529</v>
       </c>
@@ -5899,7 +5926,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -5934,7 +5961,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -5969,12 +5996,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>161</v>
       </c>
       <c r="B87" t="s">
-        <v>161</v>
+        <v>702</v>
       </c>
       <c r="C87" t="s">
         <v>369</v>
@@ -6004,12 +6031,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>171</v>
       </c>
       <c r="B88" t="s">
-        <v>171</v>
+        <v>703</v>
       </c>
       <c r="C88" t="s">
         <v>369</v>
@@ -6304,7 +6331,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>46</v>
       </c>
@@ -6441,12 +6468,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>160</v>
       </c>
       <c r="B101" t="s">
-        <v>160</v>
+        <v>707</v>
       </c>
       <c r="C101" t="s">
         <v>369</v>
@@ -6476,12 +6503,12 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>170</v>
       </c>
       <c r="B102" t="s">
-        <v>170</v>
+        <v>708</v>
       </c>
       <c r="C102" t="s">
         <v>369</v>
@@ -6945,7 +6972,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>263</v>
       </c>
@@ -7760,7 +7787,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>526</v>
       </c>
@@ -7795,7 +7822,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>527</v>
       </c>
@@ -7830,7 +7857,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>528</v>
       </c>
@@ -7865,7 +7892,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>592</v>
       </c>
@@ -7904,7 +7931,7 @@
   <autoFilter ref="A1:L144" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="UNHCR"/>
+        <filter val="ILO"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -7959,8 +7986,9 @@
     <hyperlink ref="G20" r:id="rId38" xr:uid="{E2C7D762-6A9C-4A71-B249-16FE24E9E22C}"/>
     <hyperlink ref="G98" r:id="rId39" xr:uid="{33E05C7A-54E2-451F-BB21-57C88D667C3E}"/>
     <hyperlink ref="G144" r:id="rId40" xr:uid="{9B77AE74-0E8F-4964-87D5-306E17A0CE78}"/>
+    <hyperlink ref="G14" r:id="rId41" xr:uid="{D15B5EBF-633C-4BC7-AC3E-E0CC404D1149}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix SDG data + wbcodesUN + create briefs
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB464E23-119A-41D2-9A4B-AA629B74E7F7}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79B3601B-8413-415A-A3CF-1E15689DF386}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2639,7 +2639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G14" sqref="G14"/>
+      <selection pane="topRight" activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>168</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>163</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>417</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>173</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>419</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>313</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>591</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>311</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>310</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>312</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>97</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>351</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>161</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>160</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>170</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>119</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>592</v>
       </c>
@@ -7929,9 +7929,23 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L144" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
+    <filterColumn colId="1">
       <filters>
-        <filter val="ILO"/>
+        <filter val="MNCH_ANC1"/>
+        <filter val="MNCH_ANC4"/>
+        <filter val="MNCH_BIRTH18"/>
+        <filter val="MNCH_DEMAND_FP"/>
+        <filter val="MNCH_DIARCARE"/>
+        <filter val="MNCH_ITN"/>
+        <filter val="MNCH_ITNPREG"/>
+        <filter val="MNCH_MLRACT"/>
+        <filter val="MNCH_MLRCARE"/>
+        <filter val="MNCH_MLRDIAG"/>
+        <filter val="MNCH_ORS"/>
+        <filter val="MNCH_PNCMOM"/>
+        <filter val="MNCH_PNCNB"/>
+        <filter val="MNCH_PNEUCARE"/>
+        <filter val="MNCH_SAB"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Update population data in clean data (for portal)
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642AE46E-10F8-46A9-BA4E-9E9A2C1B3094}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42C0FF8F-4EC3-405B-9992-D52F573DB919}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2244,7 +2244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2260,6 +2260,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2303,7 +2309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2327,6 +2333,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2634,11 +2642,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D30" sqref="D30"/>
+      <selection pane="topRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2702,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2775,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -2816,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -2857,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2980,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>157</v>
       </c>
@@ -3021,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -3062,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>424</v>
       </c>
@@ -3100,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>337</v>
       </c>
@@ -3138,7 +3147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>135</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -3217,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>168</v>
       </c>
@@ -3258,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>202</v>
       </c>
@@ -3299,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>308</v>
       </c>
@@ -3375,7 +3384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -3416,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>207</v>
       </c>
@@ -3457,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>368</v>
       </c>
@@ -3498,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>321</v>
       </c>
@@ -3574,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>307</v>
       </c>
@@ -3612,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>340</v>
       </c>
@@ -3650,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -3691,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -3732,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -3814,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -3855,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>320</v>
       </c>
@@ -3893,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>318</v>
       </c>
@@ -3931,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>163</v>
       </c>
@@ -3972,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -4013,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>355</v>
       </c>
@@ -4054,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>212</v>
       </c>
@@ -4133,7 +4142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>417</v>
       </c>
@@ -4174,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>532</v>
       </c>
@@ -4212,7 +4221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>317</v>
       </c>
@@ -4250,7 +4259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>219</v>
       </c>
@@ -4288,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>173</v>
       </c>
@@ -4329,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>419</v>
       </c>
@@ -4370,45 +4379,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:13" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="17" t="s">
         <v>423</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="17" t="s">
         <v>683</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="17">
         <v>4</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K44" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -4449,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>192</v>
       </c>
@@ -4490,45 +4499,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="17" t="s">
         <v>555</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="17" t="s">
         <v>602</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="18" t="s">
         <v>436</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="17">
         <v>5</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K47" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>356</v>
       </c>
@@ -4566,7 +4575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>323</v>
       </c>
@@ -4607,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>265</v>
       </c>
@@ -4648,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>591</v>
       </c>
@@ -4730,7 +4739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>258</v>
       </c>
@@ -4771,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>267</v>
       </c>
@@ -4812,7 +4821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>186</v>
       </c>
@@ -4853,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>311</v>
       </c>
@@ -4932,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>187</v>
       </c>
@@ -5011,7 +5020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>188</v>
       </c>
@@ -5134,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>422</v>
       </c>
@@ -5257,7 +5266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>421</v>
       </c>
@@ -5336,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>522</v>
       </c>
@@ -5567,7 +5576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>529</v>
       </c>
@@ -5602,7 +5611,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>530</v>
       </c>
@@ -5634,7 +5643,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>25</v>
       </c>
@@ -5730,7 +5739,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>319</v>
       </c>
@@ -5762,7 +5771,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>322</v>
       </c>
@@ -5794,7 +5803,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>351</v>
       </c>
@@ -5826,7 +5835,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -5858,7 +5867,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>23</v>
       </c>
@@ -5890,7 +5899,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>334</v>
       </c>
@@ -5925,7 +5934,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -5960,7 +5969,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -5995,7 +6004,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>161</v>
       </c>
@@ -6030,7 +6039,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -6135,7 +6144,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>373</v>
       </c>
@@ -6170,7 +6179,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -6234,7 +6243,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>35</v>
       </c>
@@ -6266,7 +6275,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>41</v>
       </c>
@@ -6298,7 +6307,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>309</v>
       </c>
@@ -6330,7 +6339,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>46</v>
       </c>
@@ -6365,7 +6374,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="98" spans="1:12" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" s="9" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>256</v>
       </c>
@@ -6400,7 +6409,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -6432,7 +6441,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>214</v>
       </c>
@@ -6467,7 +6476,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>160</v>
       </c>
@@ -6502,7 +6511,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>170</v>
       </c>
@@ -6537,7 +6546,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>363</v>
       </c>
@@ -6572,7 +6581,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>364</v>
       </c>
@@ -6607,7 +6616,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>362</v>
       </c>
@@ -6642,7 +6651,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>361</v>
       </c>
@@ -6677,7 +6686,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -6869,7 +6878,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>349</v>
       </c>
@@ -6936,7 +6945,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>261</v>
       </c>
@@ -6971,7 +6980,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>263</v>
       </c>
@@ -7038,7 +7047,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>669</v>
       </c>
@@ -7070,7 +7079,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>670</v>
       </c>
@@ -7166,7 +7175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>184</v>
       </c>
@@ -7201,7 +7210,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>182</v>
       </c>
@@ -7236,7 +7245,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>180</v>
       </c>
@@ -7338,7 +7347,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>241</v>
       </c>
@@ -7716,7 +7725,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>533</v>
       </c>
@@ -7751,7 +7760,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>534</v>
       </c>
@@ -7786,7 +7795,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>526</v>
       </c>
@@ -7821,7 +7830,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>527</v>
       </c>
@@ -7856,7 +7865,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>528</v>
       </c>
@@ -7891,7 +7900,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>592</v>
       </c>
@@ -7927,7 +7936,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L144" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L144" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Prenatal and Early Childhood"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Health"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G53" xr:uid="{2F5F9FA7-5446-47AF-A091-DD36F3BEED45}">
       <formula1>1</formula1>

</xml_diff>

<commit_message>
Summarize changes across versions
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/metadata.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniutdt-my.sharepoint.com/personal/yllohis_mail_utdt_edu/Documents/WB/Data-Portal-Brief-Generator/Data/Data_Raw/Country codes &amp; metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42C0FF8F-4EC3-405B-9992-D52F573DB919}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="13_ncr:1_{7ABC570B-9D59-4B39-A849-BD4C352BB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6B02020-6F7B-44A2-B180-89C8B059B6F2}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2647,7 +2647,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D47" sqref="D47"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2702,7 +2702,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>154</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>157</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>424</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>316</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>315</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>313</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>521</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>209</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>310</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>272</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>269</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>205</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>314</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>305</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>312</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>238</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>97</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>326</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>325</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>37</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>119</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>131</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>127</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>306</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>531</v>
       </c>
@@ -7315,7 +7315,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>52</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>62</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>66</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>70</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>74</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>78</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>82</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>86</v>
       </c>
@@ -7661,7 +7661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>90</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>123</v>
       </c>
@@ -7937,14 +7937,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L144" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="7">
+    <filterColumn colId="9">
       <filters>
-        <filter val="Prenatal and Early Childhood"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Health"/>
+        <filter val="0"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>